<commit_message>
Removed the hard coded data in the flightBooking.feature file
</commit_message>
<xml_diff>
--- a/src/test/resources/Input Data.xlsx
+++ b/src/test/resources/Input Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\eclipse-workspace\SeleniumAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DFD84C-15AA-43C8-98B8-C409D8FD2FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24094A93-AFA1-4772-A754-2B3C009E1C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,22 +42,22 @@
     <t>PNQ</t>
   </si>
   <si>
-    <t>15-01-2024</t>
-  </si>
-  <si>
     <t>DEL</t>
   </si>
   <si>
     <t>CHN</t>
   </si>
   <si>
-    <t>20-01-2024</t>
-  </si>
-  <si>
     <t>25-02-2024</t>
   </si>
   <si>
-    <t>13-02-2024</t>
+    <t>15-04-2024</t>
+  </si>
+  <si>
+    <t>20-03-2024</t>
+  </si>
+  <si>
+    <t>13-06-2024</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,18 +432,18 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -454,15 +454,15 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>

</xml_diff>